<commit_message>
nueva liga china 2025
</commit_message>
<xml_diff>
--- a/Ligas/Liga_brasil_2025.xlsx
+++ b/Ligas/Liga_brasil_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Desktop\ligas_datas\rockongo_web\Ligas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F3E5D0-93FD-4E22-83CB-8A77688840E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9657EB6-E092-47FC-BF2F-CD5BBC2665D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -4786,7 +4786,7 @@
         <v>30</v>
       </c>
       <c r="S67" t="str">
-        <f t="shared" ref="S67:S130" si="1">IF(D67 &gt; E67, "L", IF(D67 &lt; E67, "V", "E"))</f>
+        <f t="shared" ref="S67:S121" si="1">IF(D67 &gt; E67, "L", IF(D67 &lt; E67, "V", "E"))</f>
         <v>L</v>
       </c>
     </row>
@@ -8032,5 +8032,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q2:R121" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>